<commit_message>
Infer targets from NZ goals; target unit tests
Substantial enhancements to target handling and target testing.  Inference of netzero (NZ) goals (such as S1 and S2 netzero inferred from S1+S2 netzero) really helps fill in the gaps when using TPI as a benchmark.

Signed-off-by: Michael Tiemann <72577720+MichaelTiemannOSC@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/examples/data/20221025 ITR V2 Sample Data.xlsx
+++ b/examples/data/20221025 ITR V2 Sample Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michael/Dropbox/My Mac (MacBook-Pro.local)/Documents/GitHub/MichaelTiemannOSC/ITR/examples/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5C9AC68-FABA-DD4D-A524-F3345AE03629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0840F797-0E78-CB4A-8790-0B55D732BD1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="7060" windowWidth="35020" windowHeight="13220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1340" yWindow="1420" windowWidth="35020" windowHeight="13220" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Read me " sheetId="1" r:id="rId1"/>
@@ -280,6 +280,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{C4B44B23-D757-384B-A653-7950B9AF4546}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">With no S2 data, make this an S1-only target
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I39" authorId="0" shapeId="0" xr:uid="{E195F8E1-1BCB-844B-967E-CF16E87C6DB5}">
       <text>
         <r>
@@ -353,6 +387,72 @@
             <family val="2"/>
           </rPr>
           <t>Also, S1+S2+S3 should be S1+S3 (but S2 is in the noise, so OK)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G52" authorId="0" shapeId="0" xr:uid="{D38EA4C1-E72A-8C48-BC7D-B15C656DEAEE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>With no S3 data, make this an S1+S2 only target</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G83" authorId="0" shapeId="0" xr:uid="{E5BDDE4A-ED9B-1942-8733-935C1F2DC2F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Michael Tiemann:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>With no S3 data (yet), make this an S1+S2 target.</t>
         </r>
       </text>
     </comment>
@@ -4146,7 +4246,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4434,7 +4534,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4444,7 +4544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
       <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
@@ -4463,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:P87"/>
   <sheetViews>
-    <sheetView topLeftCell="A54" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView topLeftCell="A56" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60:XFD60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -8555,10 +8655,10 @@
   <dimension ref="A1:R961"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B767" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B696" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E782" sqref="E782"/>
+      <selection pane="bottomRight" activeCell="F713" sqref="F713"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
@@ -14529,7 +14629,10 @@
         <f>25967236</f>
         <v>25967236</v>
       </c>
-      <c r="O209" s="74"/>
+      <c r="O209" s="86">
+        <f>25967236</f>
+        <v>25967236</v>
+      </c>
     </row>
     <row r="210" spans="1:15">
       <c r="A210" s="107"/>
@@ -14558,7 +14661,10 @@
         <f>58106</f>
         <v>58106</v>
       </c>
-      <c r="O210" s="74"/>
+      <c r="O210" s="86">
+        <f>58106</f>
+        <v>58106</v>
+      </c>
     </row>
     <row r="211" spans="1:15">
       <c r="A211" s="107"/>
@@ -14587,7 +14693,10 @@
         <f>N209+N210</f>
         <v>26025342</v>
       </c>
-      <c r="O211" s="74"/>
+      <c r="O211" s="86">
+        <f>O209+O210</f>
+        <v>26025342</v>
+      </c>
     </row>
     <row r="212" spans="1:15">
       <c r="A212" s="107"/>
@@ -14616,7 +14725,10 @@
         <f>13769661</f>
         <v>13769661</v>
       </c>
-      <c r="O212" s="74"/>
+      <c r="O212" s="86">
+        <f>13769661</f>
+        <v>13769661</v>
+      </c>
     </row>
     <row r="213" spans="1:15">
       <c r="A213" s="107"/>
@@ -14642,7 +14754,10 @@
         <f>N211/0.77</f>
         <v>33799145.454545453</v>
       </c>
-      <c r="O213" s="74"/>
+      <c r="O213" s="86">
+        <f>O211/0.77</f>
+        <v>33799145.454545453</v>
+      </c>
     </row>
     <row r="214" spans="1:15">
       <c r="A214" s="107"/>
@@ -28977,11 +29092,26 @@
         <v>44561</v>
       </c>
       <c r="J713" s="73"/>
-      <c r="K713" s="74"/>
-      <c r="L713" s="73"/>
-      <c r="M713" s="74"/>
-      <c r="N713" s="73"/>
-      <c r="O713" s="74"/>
+      <c r="K713" s="74">
+        <f>K714*431.87/1000000</f>
+        <v>275.09193912063131</v>
+      </c>
+      <c r="L713" s="74">
+        <f>L714*431.87/1000000</f>
+        <v>291.59955525606466</v>
+      </c>
+      <c r="M713" s="74">
+        <f>M714*431.87/1000000</f>
+        <v>359.66882352941178</v>
+      </c>
+      <c r="N713" s="74">
+        <f>N714*431.87/1000000</f>
+        <v>316.52990895295898</v>
+      </c>
+      <c r="O713" s="74">
+        <f>O714*431.87/1000000</f>
+        <v>407.52659707724428</v>
+      </c>
     </row>
     <row r="714" spans="1:15">
       <c r="A714" s="107"/>
@@ -36259,6 +36389,333 @@
     </row>
   </sheetData>
   <mergeCells count="351">
+    <mergeCell ref="B73:B81"/>
+    <mergeCell ref="C73:C81"/>
+    <mergeCell ref="A124:A134"/>
+    <mergeCell ref="B124:B134"/>
+    <mergeCell ref="C124:C134"/>
+    <mergeCell ref="A149:A155"/>
+    <mergeCell ref="B149:B155"/>
+    <mergeCell ref="C149:C155"/>
+    <mergeCell ref="A57:A72"/>
+    <mergeCell ref="B57:B72"/>
+    <mergeCell ref="C57:C72"/>
+    <mergeCell ref="B106:B112"/>
+    <mergeCell ref="C106:C112"/>
+    <mergeCell ref="B113:B123"/>
+    <mergeCell ref="C113:C123"/>
+    <mergeCell ref="B100:B105"/>
+    <mergeCell ref="C100:C105"/>
+    <mergeCell ref="B82:B99"/>
+    <mergeCell ref="C82:C99"/>
+    <mergeCell ref="B139:B148"/>
+    <mergeCell ref="C139:C148"/>
+    <mergeCell ref="B135:B138"/>
+    <mergeCell ref="C135:C138"/>
+    <mergeCell ref="B162:B167"/>
+    <mergeCell ref="C162:C167"/>
+    <mergeCell ref="A221:A226"/>
+    <mergeCell ref="B221:B226"/>
+    <mergeCell ref="C221:C226"/>
+    <mergeCell ref="A209:A214"/>
+    <mergeCell ref="B209:B214"/>
+    <mergeCell ref="C209:C214"/>
+    <mergeCell ref="A168:A202"/>
+    <mergeCell ref="B168:B202"/>
+    <mergeCell ref="C168:C202"/>
+    <mergeCell ref="A823:A828"/>
+    <mergeCell ref="C426:C444"/>
+    <mergeCell ref="A347:A352"/>
+    <mergeCell ref="B347:B352"/>
+    <mergeCell ref="C347:C352"/>
+    <mergeCell ref="A308:A313"/>
+    <mergeCell ref="B308:B313"/>
+    <mergeCell ref="C308:C313"/>
+    <mergeCell ref="A366:A371"/>
+    <mergeCell ref="A395:A400"/>
+    <mergeCell ref="A420:A425"/>
+    <mergeCell ref="B320:B340"/>
+    <mergeCell ref="C320:C340"/>
+    <mergeCell ref="A359:A365"/>
+    <mergeCell ref="B359:B365"/>
+    <mergeCell ref="C359:C365"/>
+    <mergeCell ref="A372:A394"/>
+    <mergeCell ref="B372:B394"/>
+    <mergeCell ref="C372:C394"/>
+    <mergeCell ref="A401:A419"/>
+    <mergeCell ref="B401:B419"/>
+    <mergeCell ref="C401:C419"/>
+    <mergeCell ref="C722:C737"/>
+    <mergeCell ref="A661:A673"/>
+    <mergeCell ref="A817:A822"/>
+    <mergeCell ref="B817:B822"/>
+    <mergeCell ref="C817:C822"/>
+    <mergeCell ref="A674:A679"/>
+    <mergeCell ref="A680:A685"/>
+    <mergeCell ref="A692:A697"/>
+    <mergeCell ref="A686:A691"/>
+    <mergeCell ref="A793:A798"/>
+    <mergeCell ref="A799:A804"/>
+    <mergeCell ref="A805:A810"/>
+    <mergeCell ref="A811:A816"/>
+    <mergeCell ref="B710:B715"/>
+    <mergeCell ref="B716:B721"/>
+    <mergeCell ref="B738:B743"/>
+    <mergeCell ref="B744:B749"/>
+    <mergeCell ref="B768:B786"/>
+    <mergeCell ref="B787:B792"/>
+    <mergeCell ref="B793:B798"/>
+    <mergeCell ref="B799:B804"/>
+    <mergeCell ref="C633:C638"/>
+    <mergeCell ref="A609:A614"/>
+    <mergeCell ref="B609:B614"/>
+    <mergeCell ref="C609:C614"/>
+    <mergeCell ref="A531:A536"/>
+    <mergeCell ref="B531:B536"/>
+    <mergeCell ref="C531:C536"/>
+    <mergeCell ref="A944:A949"/>
+    <mergeCell ref="B944:B949"/>
+    <mergeCell ref="C944:C949"/>
+    <mergeCell ref="A537:A541"/>
+    <mergeCell ref="A542:A547"/>
+    <mergeCell ref="A548:A553"/>
+    <mergeCell ref="A561:A566"/>
+    <mergeCell ref="A567:A572"/>
+    <mergeCell ref="A573:A578"/>
+    <mergeCell ref="A579:A584"/>
+    <mergeCell ref="A585:A590"/>
+    <mergeCell ref="A591:A596"/>
+    <mergeCell ref="A597:A602"/>
+    <mergeCell ref="A603:A608"/>
+    <mergeCell ref="A615:A632"/>
+    <mergeCell ref="A639:A654"/>
+    <mergeCell ref="A655:A660"/>
+    <mergeCell ref="A271:A283"/>
+    <mergeCell ref="A31:A40"/>
+    <mergeCell ref="A284:A289"/>
+    <mergeCell ref="A290:A295"/>
+    <mergeCell ref="A296:A301"/>
+    <mergeCell ref="A302:A307"/>
+    <mergeCell ref="A314:A319"/>
+    <mergeCell ref="A341:A346"/>
+    <mergeCell ref="A353:A358"/>
+    <mergeCell ref="A162:A167"/>
+    <mergeCell ref="A73:A81"/>
+    <mergeCell ref="A106:A112"/>
+    <mergeCell ref="A113:A123"/>
+    <mergeCell ref="A100:A105"/>
+    <mergeCell ref="A82:A99"/>
+    <mergeCell ref="A139:A148"/>
+    <mergeCell ref="A135:A138"/>
+    <mergeCell ref="A320:A340"/>
+    <mergeCell ref="A445:A450"/>
+    <mergeCell ref="A476:A481"/>
+    <mergeCell ref="A482:A487"/>
+    <mergeCell ref="A488:A493"/>
+    <mergeCell ref="A507:A512"/>
+    <mergeCell ref="A519:A524"/>
+    <mergeCell ref="A513:A518"/>
+    <mergeCell ref="A426:A444"/>
+    <mergeCell ref="A525:A530"/>
+    <mergeCell ref="A451:A475"/>
+    <mergeCell ref="A633:A638"/>
+    <mergeCell ref="A698:A703"/>
+    <mergeCell ref="A704:A709"/>
+    <mergeCell ref="A710:A715"/>
+    <mergeCell ref="A716:A721"/>
+    <mergeCell ref="A738:A743"/>
+    <mergeCell ref="A744:A749"/>
+    <mergeCell ref="A768:A786"/>
+    <mergeCell ref="A787:A792"/>
+    <mergeCell ref="A762:A767"/>
+    <mergeCell ref="A722:A737"/>
+    <mergeCell ref="A750:A761"/>
+    <mergeCell ref="A890:A895"/>
+    <mergeCell ref="A896:A901"/>
+    <mergeCell ref="A902:A907"/>
+    <mergeCell ref="A908:A913"/>
+    <mergeCell ref="A914:A919"/>
+    <mergeCell ref="A920:A925"/>
+    <mergeCell ref="A926:A931"/>
+    <mergeCell ref="A932:A937"/>
+    <mergeCell ref="A829:A834"/>
+    <mergeCell ref="A835:A840"/>
+    <mergeCell ref="A847:A853"/>
+    <mergeCell ref="A854:A859"/>
+    <mergeCell ref="A860:A865"/>
+    <mergeCell ref="A841:A846"/>
+    <mergeCell ref="A866:A871"/>
+    <mergeCell ref="A872:A877"/>
+    <mergeCell ref="A878:A883"/>
+    <mergeCell ref="A950:A955"/>
+    <mergeCell ref="A956:A961"/>
+    <mergeCell ref="B21:B30"/>
+    <mergeCell ref="B41:B56"/>
+    <mergeCell ref="B156:B161"/>
+    <mergeCell ref="B203:B208"/>
+    <mergeCell ref="B215:B220"/>
+    <mergeCell ref="B227:B232"/>
+    <mergeCell ref="B233:B238"/>
+    <mergeCell ref="B239:B244"/>
+    <mergeCell ref="B271:B283"/>
+    <mergeCell ref="B284:B289"/>
+    <mergeCell ref="B290:B295"/>
+    <mergeCell ref="B296:B301"/>
+    <mergeCell ref="B302:B307"/>
+    <mergeCell ref="B314:B319"/>
+    <mergeCell ref="B341:B346"/>
+    <mergeCell ref="B353:B358"/>
+    <mergeCell ref="B366:B371"/>
+    <mergeCell ref="B395:B400"/>
+    <mergeCell ref="B420:B425"/>
+    <mergeCell ref="B445:B450"/>
+    <mergeCell ref="B476:B481"/>
+    <mergeCell ref="A884:A889"/>
+    <mergeCell ref="B482:B487"/>
+    <mergeCell ref="B488:B493"/>
+    <mergeCell ref="B507:B512"/>
+    <mergeCell ref="B519:B524"/>
+    <mergeCell ref="B525:B530"/>
+    <mergeCell ref="B537:B541"/>
+    <mergeCell ref="B513:B518"/>
+    <mergeCell ref="B426:B444"/>
+    <mergeCell ref="B542:B547"/>
+    <mergeCell ref="B451:B475"/>
+    <mergeCell ref="B548:B553"/>
+    <mergeCell ref="B561:B566"/>
+    <mergeCell ref="B567:B572"/>
+    <mergeCell ref="B573:B578"/>
+    <mergeCell ref="B579:B584"/>
+    <mergeCell ref="B585:B590"/>
+    <mergeCell ref="B591:B596"/>
+    <mergeCell ref="B597:B602"/>
+    <mergeCell ref="B603:B608"/>
+    <mergeCell ref="B615:B632"/>
+    <mergeCell ref="B639:B654"/>
+    <mergeCell ref="B655:B660"/>
+    <mergeCell ref="B674:B679"/>
+    <mergeCell ref="B680:B685"/>
+    <mergeCell ref="B692:B697"/>
+    <mergeCell ref="B698:B703"/>
+    <mergeCell ref="B704:B709"/>
+    <mergeCell ref="B686:B691"/>
+    <mergeCell ref="B633:B638"/>
+    <mergeCell ref="B661:B673"/>
+    <mergeCell ref="B805:B810"/>
+    <mergeCell ref="B762:B767"/>
+    <mergeCell ref="B722:B737"/>
+    <mergeCell ref="B884:B889"/>
+    <mergeCell ref="B890:B895"/>
+    <mergeCell ref="B896:B901"/>
+    <mergeCell ref="B902:B907"/>
+    <mergeCell ref="B908:B913"/>
+    <mergeCell ref="B914:B919"/>
+    <mergeCell ref="B750:B761"/>
+    <mergeCell ref="B920:B925"/>
+    <mergeCell ref="B926:B931"/>
+    <mergeCell ref="B811:B816"/>
+    <mergeCell ref="B823:B828"/>
+    <mergeCell ref="B829:B834"/>
+    <mergeCell ref="B835:B840"/>
+    <mergeCell ref="B847:B853"/>
+    <mergeCell ref="B854:B859"/>
+    <mergeCell ref="B860:B865"/>
+    <mergeCell ref="B866:B871"/>
+    <mergeCell ref="B872:B877"/>
+    <mergeCell ref="B841:B846"/>
+    <mergeCell ref="B932:B937"/>
+    <mergeCell ref="B950:B955"/>
+    <mergeCell ref="B956:B961"/>
+    <mergeCell ref="C21:C30"/>
+    <mergeCell ref="C41:C56"/>
+    <mergeCell ref="C156:C161"/>
+    <mergeCell ref="C203:C208"/>
+    <mergeCell ref="C215:C220"/>
+    <mergeCell ref="C227:C232"/>
+    <mergeCell ref="C233:C238"/>
+    <mergeCell ref="C239:C244"/>
+    <mergeCell ref="C271:C283"/>
+    <mergeCell ref="C284:C289"/>
+    <mergeCell ref="C290:C295"/>
+    <mergeCell ref="C296:C301"/>
+    <mergeCell ref="C302:C307"/>
+    <mergeCell ref="C314:C319"/>
+    <mergeCell ref="C341:C346"/>
+    <mergeCell ref="C353:C358"/>
+    <mergeCell ref="C366:C371"/>
+    <mergeCell ref="C395:C400"/>
+    <mergeCell ref="C420:C425"/>
+    <mergeCell ref="C445:C450"/>
+    <mergeCell ref="B878:B883"/>
+    <mergeCell ref="C476:C481"/>
+    <mergeCell ref="C482:C487"/>
+    <mergeCell ref="C488:C493"/>
+    <mergeCell ref="C507:C512"/>
+    <mergeCell ref="C519:C524"/>
+    <mergeCell ref="C525:C530"/>
+    <mergeCell ref="C537:C541"/>
+    <mergeCell ref="C542:C547"/>
+    <mergeCell ref="C548:C553"/>
+    <mergeCell ref="C513:C518"/>
+    <mergeCell ref="C561:C566"/>
+    <mergeCell ref="C567:C572"/>
+    <mergeCell ref="C573:C578"/>
+    <mergeCell ref="C579:C584"/>
+    <mergeCell ref="C585:C590"/>
+    <mergeCell ref="C591:C596"/>
+    <mergeCell ref="C597:C602"/>
+    <mergeCell ref="C603:C608"/>
+    <mergeCell ref="C615:C632"/>
+    <mergeCell ref="C639:C654"/>
+    <mergeCell ref="C655:C660"/>
+    <mergeCell ref="C674:C679"/>
+    <mergeCell ref="C680:C685"/>
+    <mergeCell ref="C692:C697"/>
+    <mergeCell ref="C698:C703"/>
+    <mergeCell ref="C704:C709"/>
+    <mergeCell ref="C710:C715"/>
+    <mergeCell ref="C716:C721"/>
+    <mergeCell ref="C686:C691"/>
+    <mergeCell ref="C661:C673"/>
+    <mergeCell ref="C872:C877"/>
+    <mergeCell ref="C878:C883"/>
+    <mergeCell ref="C884:C889"/>
+    <mergeCell ref="C841:C846"/>
+    <mergeCell ref="C738:C743"/>
+    <mergeCell ref="C744:C749"/>
+    <mergeCell ref="C768:C786"/>
+    <mergeCell ref="C787:C792"/>
+    <mergeCell ref="C793:C798"/>
+    <mergeCell ref="C799:C804"/>
+    <mergeCell ref="C805:C810"/>
+    <mergeCell ref="C811:C816"/>
+    <mergeCell ref="C823:C828"/>
+    <mergeCell ref="C762:C767"/>
+    <mergeCell ref="C750:C761"/>
+    <mergeCell ref="C950:C955"/>
+    <mergeCell ref="C956:C961"/>
+    <mergeCell ref="B31:B40"/>
+    <mergeCell ref="C31:C40"/>
+    <mergeCell ref="A11:A20"/>
+    <mergeCell ref="B11:B20"/>
+    <mergeCell ref="C11:C20"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="C2:C10"/>
+    <mergeCell ref="A258:A270"/>
+    <mergeCell ref="B258:B270"/>
+    <mergeCell ref="C258:C270"/>
+    <mergeCell ref="A245:A257"/>
+    <mergeCell ref="B245:B257"/>
+    <mergeCell ref="C245:C257"/>
+    <mergeCell ref="A21:A30"/>
+    <mergeCell ref="A41:A56"/>
+    <mergeCell ref="A156:A161"/>
+    <mergeCell ref="A203:A208"/>
+    <mergeCell ref="A215:A220"/>
+    <mergeCell ref="A227:A232"/>
+    <mergeCell ref="A233:A238"/>
+    <mergeCell ref="A239:A244"/>
     <mergeCell ref="C451:C475"/>
     <mergeCell ref="A494:A506"/>
     <mergeCell ref="B494:B506"/>
@@ -36283,333 +36740,6 @@
     <mergeCell ref="C854:C859"/>
     <mergeCell ref="C860:C865"/>
     <mergeCell ref="C866:C871"/>
-    <mergeCell ref="C950:C955"/>
-    <mergeCell ref="C956:C961"/>
-    <mergeCell ref="B31:B40"/>
-    <mergeCell ref="C31:C40"/>
-    <mergeCell ref="A11:A20"/>
-    <mergeCell ref="B11:B20"/>
-    <mergeCell ref="C11:C20"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="B2:B10"/>
-    <mergeCell ref="C2:C10"/>
-    <mergeCell ref="A258:A270"/>
-    <mergeCell ref="B258:B270"/>
-    <mergeCell ref="C258:C270"/>
-    <mergeCell ref="A245:A257"/>
-    <mergeCell ref="B245:B257"/>
-    <mergeCell ref="C245:C257"/>
-    <mergeCell ref="A21:A30"/>
-    <mergeCell ref="A41:A56"/>
-    <mergeCell ref="A156:A161"/>
-    <mergeCell ref="A203:A208"/>
-    <mergeCell ref="A215:A220"/>
-    <mergeCell ref="A227:A232"/>
-    <mergeCell ref="A233:A238"/>
-    <mergeCell ref="A239:A244"/>
-    <mergeCell ref="C872:C877"/>
-    <mergeCell ref="C878:C883"/>
-    <mergeCell ref="C884:C889"/>
-    <mergeCell ref="C841:C846"/>
-    <mergeCell ref="C738:C743"/>
-    <mergeCell ref="C744:C749"/>
-    <mergeCell ref="C768:C786"/>
-    <mergeCell ref="C787:C792"/>
-    <mergeCell ref="C793:C798"/>
-    <mergeCell ref="C799:C804"/>
-    <mergeCell ref="C805:C810"/>
-    <mergeCell ref="C811:C816"/>
-    <mergeCell ref="C823:C828"/>
-    <mergeCell ref="C762:C767"/>
-    <mergeCell ref="C639:C654"/>
-    <mergeCell ref="C655:C660"/>
-    <mergeCell ref="C674:C679"/>
-    <mergeCell ref="C680:C685"/>
-    <mergeCell ref="C692:C697"/>
-    <mergeCell ref="C698:C703"/>
-    <mergeCell ref="C704:C709"/>
-    <mergeCell ref="C710:C715"/>
-    <mergeCell ref="C716:C721"/>
-    <mergeCell ref="C686:C691"/>
-    <mergeCell ref="C561:C566"/>
-    <mergeCell ref="C567:C572"/>
-    <mergeCell ref="C573:C578"/>
-    <mergeCell ref="C579:C584"/>
-    <mergeCell ref="C585:C590"/>
-    <mergeCell ref="C591:C596"/>
-    <mergeCell ref="C597:C602"/>
-    <mergeCell ref="C603:C608"/>
-    <mergeCell ref="C615:C632"/>
-    <mergeCell ref="C476:C481"/>
-    <mergeCell ref="C482:C487"/>
-    <mergeCell ref="C488:C493"/>
-    <mergeCell ref="C507:C512"/>
-    <mergeCell ref="C519:C524"/>
-    <mergeCell ref="C525:C530"/>
-    <mergeCell ref="C537:C541"/>
-    <mergeCell ref="C542:C547"/>
-    <mergeCell ref="C548:C553"/>
-    <mergeCell ref="C513:C518"/>
-    <mergeCell ref="B932:B937"/>
-    <mergeCell ref="B950:B955"/>
-    <mergeCell ref="B956:B961"/>
-    <mergeCell ref="C21:C30"/>
-    <mergeCell ref="C41:C56"/>
-    <mergeCell ref="C156:C161"/>
-    <mergeCell ref="C203:C208"/>
-    <mergeCell ref="C215:C220"/>
-    <mergeCell ref="C227:C232"/>
-    <mergeCell ref="C233:C238"/>
-    <mergeCell ref="C239:C244"/>
-    <mergeCell ref="C271:C283"/>
-    <mergeCell ref="C284:C289"/>
-    <mergeCell ref="C290:C295"/>
-    <mergeCell ref="C296:C301"/>
-    <mergeCell ref="C302:C307"/>
-    <mergeCell ref="C314:C319"/>
-    <mergeCell ref="C341:C346"/>
-    <mergeCell ref="C353:C358"/>
-    <mergeCell ref="C366:C371"/>
-    <mergeCell ref="C395:C400"/>
-    <mergeCell ref="C420:C425"/>
-    <mergeCell ref="C445:C450"/>
-    <mergeCell ref="B878:B883"/>
-    <mergeCell ref="B920:B925"/>
-    <mergeCell ref="B926:B931"/>
-    <mergeCell ref="B811:B816"/>
-    <mergeCell ref="B823:B828"/>
-    <mergeCell ref="B829:B834"/>
-    <mergeCell ref="B835:B840"/>
-    <mergeCell ref="B847:B853"/>
-    <mergeCell ref="B854:B859"/>
-    <mergeCell ref="B860:B865"/>
-    <mergeCell ref="B866:B871"/>
-    <mergeCell ref="B872:B877"/>
-    <mergeCell ref="B841:B846"/>
-    <mergeCell ref="B805:B810"/>
-    <mergeCell ref="B762:B767"/>
-    <mergeCell ref="B722:B737"/>
-    <mergeCell ref="B884:B889"/>
-    <mergeCell ref="B890:B895"/>
-    <mergeCell ref="B896:B901"/>
-    <mergeCell ref="B902:B907"/>
-    <mergeCell ref="B908:B913"/>
-    <mergeCell ref="B914:B919"/>
-    <mergeCell ref="B615:B632"/>
-    <mergeCell ref="B639:B654"/>
-    <mergeCell ref="B655:B660"/>
-    <mergeCell ref="B674:B679"/>
-    <mergeCell ref="B680:B685"/>
-    <mergeCell ref="B692:B697"/>
-    <mergeCell ref="B698:B703"/>
-    <mergeCell ref="B704:B709"/>
-    <mergeCell ref="B686:B691"/>
-    <mergeCell ref="B633:B638"/>
-    <mergeCell ref="B548:B553"/>
-    <mergeCell ref="B561:B566"/>
-    <mergeCell ref="B567:B572"/>
-    <mergeCell ref="B573:B578"/>
-    <mergeCell ref="B579:B584"/>
-    <mergeCell ref="B585:B590"/>
-    <mergeCell ref="B591:B596"/>
-    <mergeCell ref="B597:B602"/>
-    <mergeCell ref="B603:B608"/>
-    <mergeCell ref="B482:B487"/>
-    <mergeCell ref="B488:B493"/>
-    <mergeCell ref="B507:B512"/>
-    <mergeCell ref="B519:B524"/>
-    <mergeCell ref="B525:B530"/>
-    <mergeCell ref="B537:B541"/>
-    <mergeCell ref="B513:B518"/>
-    <mergeCell ref="B426:B444"/>
-    <mergeCell ref="B542:B547"/>
-    <mergeCell ref="B451:B475"/>
-    <mergeCell ref="A950:A955"/>
-    <mergeCell ref="A956:A961"/>
-    <mergeCell ref="B21:B30"/>
-    <mergeCell ref="B41:B56"/>
-    <mergeCell ref="B156:B161"/>
-    <mergeCell ref="B203:B208"/>
-    <mergeCell ref="B215:B220"/>
-    <mergeCell ref="B227:B232"/>
-    <mergeCell ref="B233:B238"/>
-    <mergeCell ref="B239:B244"/>
-    <mergeCell ref="B271:B283"/>
-    <mergeCell ref="B284:B289"/>
-    <mergeCell ref="B290:B295"/>
-    <mergeCell ref="B296:B301"/>
-    <mergeCell ref="B302:B307"/>
-    <mergeCell ref="B314:B319"/>
-    <mergeCell ref="B341:B346"/>
-    <mergeCell ref="B353:B358"/>
-    <mergeCell ref="B366:B371"/>
-    <mergeCell ref="B395:B400"/>
-    <mergeCell ref="B420:B425"/>
-    <mergeCell ref="B445:B450"/>
-    <mergeCell ref="B476:B481"/>
-    <mergeCell ref="A884:A889"/>
-    <mergeCell ref="A890:A895"/>
-    <mergeCell ref="A896:A901"/>
-    <mergeCell ref="A902:A907"/>
-    <mergeCell ref="A908:A913"/>
-    <mergeCell ref="A914:A919"/>
-    <mergeCell ref="A920:A925"/>
-    <mergeCell ref="A926:A931"/>
-    <mergeCell ref="A932:A937"/>
-    <mergeCell ref="A829:A834"/>
-    <mergeCell ref="A835:A840"/>
-    <mergeCell ref="A847:A853"/>
-    <mergeCell ref="A854:A859"/>
-    <mergeCell ref="A860:A865"/>
-    <mergeCell ref="A841:A846"/>
-    <mergeCell ref="A866:A871"/>
-    <mergeCell ref="A872:A877"/>
-    <mergeCell ref="A878:A883"/>
-    <mergeCell ref="A633:A638"/>
-    <mergeCell ref="A698:A703"/>
-    <mergeCell ref="A704:A709"/>
-    <mergeCell ref="A710:A715"/>
-    <mergeCell ref="A716:A721"/>
-    <mergeCell ref="A738:A743"/>
-    <mergeCell ref="A744:A749"/>
-    <mergeCell ref="A768:A786"/>
-    <mergeCell ref="A787:A792"/>
-    <mergeCell ref="A762:A767"/>
-    <mergeCell ref="A722:A737"/>
-    <mergeCell ref="A445:A450"/>
-    <mergeCell ref="A476:A481"/>
-    <mergeCell ref="A482:A487"/>
-    <mergeCell ref="A488:A493"/>
-    <mergeCell ref="A507:A512"/>
-    <mergeCell ref="A519:A524"/>
-    <mergeCell ref="A513:A518"/>
-    <mergeCell ref="A426:A444"/>
-    <mergeCell ref="A525:A530"/>
-    <mergeCell ref="A451:A475"/>
-    <mergeCell ref="A271:A283"/>
-    <mergeCell ref="A31:A40"/>
-    <mergeCell ref="A284:A289"/>
-    <mergeCell ref="A290:A295"/>
-    <mergeCell ref="A296:A301"/>
-    <mergeCell ref="A302:A307"/>
-    <mergeCell ref="A314:A319"/>
-    <mergeCell ref="A341:A346"/>
-    <mergeCell ref="A353:A358"/>
-    <mergeCell ref="A162:A167"/>
-    <mergeCell ref="A73:A81"/>
-    <mergeCell ref="A106:A112"/>
-    <mergeCell ref="A113:A123"/>
-    <mergeCell ref="A100:A105"/>
-    <mergeCell ref="A82:A99"/>
-    <mergeCell ref="A139:A148"/>
-    <mergeCell ref="A135:A138"/>
-    <mergeCell ref="A320:A340"/>
-    <mergeCell ref="C633:C638"/>
-    <mergeCell ref="A609:A614"/>
-    <mergeCell ref="B609:B614"/>
-    <mergeCell ref="C609:C614"/>
-    <mergeCell ref="A531:A536"/>
-    <mergeCell ref="B531:B536"/>
-    <mergeCell ref="C531:C536"/>
-    <mergeCell ref="A944:A949"/>
-    <mergeCell ref="B944:B949"/>
-    <mergeCell ref="C944:C949"/>
-    <mergeCell ref="A537:A541"/>
-    <mergeCell ref="A542:A547"/>
-    <mergeCell ref="A548:A553"/>
-    <mergeCell ref="A561:A566"/>
-    <mergeCell ref="A567:A572"/>
-    <mergeCell ref="A573:A578"/>
-    <mergeCell ref="A579:A584"/>
-    <mergeCell ref="A585:A590"/>
-    <mergeCell ref="A591:A596"/>
-    <mergeCell ref="A597:A602"/>
-    <mergeCell ref="A603:A608"/>
-    <mergeCell ref="A615:A632"/>
-    <mergeCell ref="A639:A654"/>
-    <mergeCell ref="A655:A660"/>
-    <mergeCell ref="B661:B673"/>
-    <mergeCell ref="C661:C673"/>
-    <mergeCell ref="A750:A761"/>
-    <mergeCell ref="B750:B761"/>
-    <mergeCell ref="C750:C761"/>
-    <mergeCell ref="A817:A822"/>
-    <mergeCell ref="B817:B822"/>
-    <mergeCell ref="C817:C822"/>
-    <mergeCell ref="A674:A679"/>
-    <mergeCell ref="A680:A685"/>
-    <mergeCell ref="A692:A697"/>
-    <mergeCell ref="A686:A691"/>
-    <mergeCell ref="A793:A798"/>
-    <mergeCell ref="A799:A804"/>
-    <mergeCell ref="A805:A810"/>
-    <mergeCell ref="A811:A816"/>
-    <mergeCell ref="B710:B715"/>
-    <mergeCell ref="B716:B721"/>
-    <mergeCell ref="B738:B743"/>
-    <mergeCell ref="B744:B749"/>
-    <mergeCell ref="B768:B786"/>
-    <mergeCell ref="B787:B792"/>
-    <mergeCell ref="B793:B798"/>
-    <mergeCell ref="B799:B804"/>
-    <mergeCell ref="A823:A828"/>
-    <mergeCell ref="C426:C444"/>
-    <mergeCell ref="A347:A352"/>
-    <mergeCell ref="B347:B352"/>
-    <mergeCell ref="C347:C352"/>
-    <mergeCell ref="A308:A313"/>
-    <mergeCell ref="B308:B313"/>
-    <mergeCell ref="C308:C313"/>
-    <mergeCell ref="A366:A371"/>
-    <mergeCell ref="A395:A400"/>
-    <mergeCell ref="A420:A425"/>
-    <mergeCell ref="B320:B340"/>
-    <mergeCell ref="C320:C340"/>
-    <mergeCell ref="A359:A365"/>
-    <mergeCell ref="B359:B365"/>
-    <mergeCell ref="C359:C365"/>
-    <mergeCell ref="A372:A394"/>
-    <mergeCell ref="B372:B394"/>
-    <mergeCell ref="C372:C394"/>
-    <mergeCell ref="A401:A419"/>
-    <mergeCell ref="B401:B419"/>
-    <mergeCell ref="C401:C419"/>
-    <mergeCell ref="C722:C737"/>
-    <mergeCell ref="A661:A673"/>
-    <mergeCell ref="B162:B167"/>
-    <mergeCell ref="C162:C167"/>
-    <mergeCell ref="A221:A226"/>
-    <mergeCell ref="B221:B226"/>
-    <mergeCell ref="C221:C226"/>
-    <mergeCell ref="A209:A214"/>
-    <mergeCell ref="B209:B214"/>
-    <mergeCell ref="C209:C214"/>
-    <mergeCell ref="A168:A202"/>
-    <mergeCell ref="B168:B202"/>
-    <mergeCell ref="C168:C202"/>
-    <mergeCell ref="B73:B81"/>
-    <mergeCell ref="C73:C81"/>
-    <mergeCell ref="A124:A134"/>
-    <mergeCell ref="B124:B134"/>
-    <mergeCell ref="C124:C134"/>
-    <mergeCell ref="A149:A155"/>
-    <mergeCell ref="B149:B155"/>
-    <mergeCell ref="C149:C155"/>
-    <mergeCell ref="A57:A72"/>
-    <mergeCell ref="B57:B72"/>
-    <mergeCell ref="C57:C72"/>
-    <mergeCell ref="B106:B112"/>
-    <mergeCell ref="C106:C112"/>
-    <mergeCell ref="B113:B123"/>
-    <mergeCell ref="C113:C123"/>
-    <mergeCell ref="B100:B105"/>
-    <mergeCell ref="C100:C105"/>
-    <mergeCell ref="B82:B99"/>
-    <mergeCell ref="C82:C99"/>
-    <mergeCell ref="B139:B148"/>
-    <mergeCell ref="C139:C148"/>
-    <mergeCell ref="B135:B138"/>
-    <mergeCell ref="C135:C138"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="N30" r:id="rId1" xr:uid="{0B00E541-600E-124F-8530-7CF03623D698}"/>
@@ -38000,10 +38130,10 @@
   <dimension ref="A1:O129"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
-      <selection pane="bottomRight" activeCell="B102" sqref="B102"/>
+      <selection pane="bottomRight" activeCell="G126" sqref="G126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -38179,7 +38309,7 @@
         <v>2016</v>
       </c>
       <c r="J4">
-        <v>0.67</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="K4" t="s">
         <v>436</v>
@@ -39279,7 +39409,7 @@
         <v>332</v>
       </c>
       <c r="G31" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="I31" s="57">
         <v>2011</v>
@@ -40181,7 +40311,7 @@
         <v>332</v>
       </c>
       <c r="G52" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H52">
         <v>2020</v>
@@ -41420,7 +41550,7 @@
         <v>332</v>
       </c>
       <c r="G83" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="H83">
         <v>2021</v>
@@ -43179,7 +43309,7 @@
         <v>330</v>
       </c>
       <c r="G126" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="H126">
         <v>2020</v>
@@ -44947,8 +45077,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E77"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView topLeftCell="A8" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
@@ -44990,7 +45120,7 @@
       </c>
       <c r="E2">
         <f t="shared" ref="E2:E33" ca="1" si="0">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>157979037</v>
+        <v>142727728</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -45008,7 +45138,7 @@
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="0"/>
-        <v>155034737</v>
+        <v>80347498</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -45026,7 +45156,7 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>134078500</v>
+        <v>57197626</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -45044,7 +45174,7 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>263390880</v>
+        <v>154935804</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -45062,7 +45192,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>166573482</v>
+        <v>162100932</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -45080,7 +45210,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>65472138</v>
+        <v>162033428</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -45098,7 +45228,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>160950634</v>
+        <v>52997670</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -45116,7 +45246,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>249962560</v>
+        <v>117303606</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -45134,7 +45264,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>75412281</v>
+        <v>69013800</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -45152,7 +45282,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>69891264</v>
+        <v>233186187</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -45170,7 +45300,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>257677915</v>
+        <v>143495990</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -45188,7 +45318,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>227983120</v>
+        <v>234129980</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -45206,7 +45336,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>198419375</v>
+        <v>89116122</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -45224,7 +45354,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>82026285</v>
+        <v>91498511</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -45242,7 +45372,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>120083648</v>
+        <v>94210230</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -45260,7 +45390,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>84940317</v>
+        <v>159749172</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -45278,7 +45408,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>72375699</v>
+        <v>61618752</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -45296,7 +45426,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>129053136</v>
+        <v>71815212</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -45314,7 +45444,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>112733726</v>
+        <v>63539712</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -45332,7 +45462,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>274620816</v>
+        <v>85995225</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -45350,7 +45480,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>59809078</v>
+        <v>69522024</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -45368,7 +45498,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>131805484</v>
+        <v>57166560</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -45386,7 +45516,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>212026470</v>
+        <v>71184132</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -45404,7 +45534,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>162776151</v>
+        <v>112684940</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -45422,7 +45552,7 @@
       </c>
       <c r="E26">
         <f t="shared" ca="1" si="0"/>
-        <v>62624712</v>
+        <v>141044400</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -45440,7 +45570,7 @@
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="0"/>
-        <v>161494798</v>
+        <v>118511442</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -45458,7 +45588,7 @@
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>173369745</v>
+        <v>88834208</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -45476,7 +45606,7 @@
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="0"/>
-        <v>127169224</v>
+        <v>224899850</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -45494,7 +45624,7 @@
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="0"/>
-        <v>203583878</v>
+        <v>130275000</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -45512,7 +45642,7 @@
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="0"/>
-        <v>240626142</v>
+        <v>75490392</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -45530,7 +45660,7 @@
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="0"/>
-        <v>214749296</v>
+        <v>196090488</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -45548,7 +45678,7 @@
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="0"/>
-        <v>110821801</v>
+        <v>144787032</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -45566,7 +45696,7 @@
       </c>
       <c r="E34">
         <f t="shared" ref="E34:E65" ca="1" si="1">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>138920731</v>
+        <v>140410627</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -45584,7 +45714,7 @@
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="1"/>
-        <v>55410711</v>
+        <v>57750406</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -45602,7 +45732,7 @@
       </c>
       <c r="E36">
         <f t="shared" ca="1" si="1"/>
-        <v>69536610</v>
+        <v>92958855</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -45620,7 +45750,7 @@
       </c>
       <c r="E37">
         <f t="shared" ca="1" si="1"/>
-        <v>100306472</v>
+        <v>35804106</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -45638,7 +45768,7 @@
       </c>
       <c r="E38">
         <f t="shared" ca="1" si="1"/>
-        <v>117159490</v>
+        <v>169118808</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -45656,7 +45786,7 @@
       </c>
       <c r="E39">
         <f t="shared" ca="1" si="1"/>
-        <v>274938136</v>
+        <v>187819632</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -45674,7 +45804,7 @@
       </c>
       <c r="E40">
         <f t="shared" ca="1" si="1"/>
-        <v>112182954</v>
+        <v>148662180</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -45692,7 +45822,7 @@
       </c>
       <c r="E41">
         <f t="shared" ca="1" si="1"/>
-        <v>172207425</v>
+        <v>149916000</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -45710,7 +45840,7 @@
       </c>
       <c r="E42">
         <f t="shared" ca="1" si="1"/>
-        <v>242310332</v>
+        <v>253798272</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -45728,7 +45858,7 @@
       </c>
       <c r="E43">
         <f t="shared" ca="1" si="1"/>
-        <v>186376881</v>
+        <v>113283065</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -45746,7 +45876,7 @@
       </c>
       <c r="E44">
         <f t="shared" ca="1" si="1"/>
-        <v>113699256</v>
+        <v>136331475</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -45764,7 +45894,7 @@
       </c>
       <c r="E45">
         <f t="shared" ca="1" si="1"/>
-        <v>97205480</v>
+        <v>93770386</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -45782,7 +45912,7 @@
       </c>
       <c r="E46">
         <f t="shared" ca="1" si="1"/>
-        <v>71120907</v>
+        <v>83236779</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -45800,7 +45930,7 @@
       </c>
       <c r="E47">
         <f t="shared" ca="1" si="1"/>
-        <v>180893430</v>
+        <v>126107225</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -45818,7 +45948,7 @@
       </c>
       <c r="E48">
         <f t="shared" ca="1" si="1"/>
-        <v>151184469</v>
+        <v>54100059</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -45836,7 +45966,7 @@
       </c>
       <c r="E49">
         <f t="shared" ca="1" si="1"/>
-        <v>95149125</v>
+        <v>67054982</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -45854,7 +45984,7 @@
       </c>
       <c r="E50">
         <f t="shared" ca="1" si="1"/>
-        <v>139338738</v>
+        <v>66987266</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -45872,7 +46002,7 @@
       </c>
       <c r="E51">
         <f t="shared" ca="1" si="1"/>
-        <v>85970364</v>
+        <v>105235859</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -45890,7 +46020,7 @@
       </c>
       <c r="E52">
         <f t="shared" ca="1" si="1"/>
-        <v>60470766</v>
+        <v>75395528</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -45908,7 +46038,7 @@
       </c>
       <c r="E53">
         <f t="shared" ca="1" si="1"/>
-        <v>132179213</v>
+        <v>105134310</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -45926,7 +46056,7 @@
       </c>
       <c r="E54">
         <f t="shared" ca="1" si="1"/>
-        <v>57905848</v>
+        <v>108755528</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -45944,7 +46074,7 @@
       </c>
       <c r="E55">
         <f t="shared" ca="1" si="1"/>
-        <v>101584704</v>
+        <v>160195810</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -45962,7 +46092,7 @@
       </c>
       <c r="E56">
         <f t="shared" ca="1" si="1"/>
-        <v>218380030</v>
+        <v>104944059</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -45980,7 +46110,7 @@
       </c>
       <c r="E57">
         <f t="shared" ca="1" si="1"/>
-        <v>93590588</v>
+        <v>90061032</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -45998,7 +46128,7 @@
       </c>
       <c r="E58">
         <f t="shared" ca="1" si="1"/>
-        <v>114619348</v>
+        <v>181100582</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -46016,7 +46146,7 @@
       </c>
       <c r="E59">
         <f t="shared" ca="1" si="1"/>
-        <v>164063146</v>
+        <v>160246971</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -46034,7 +46164,7 @@
       </c>
       <c r="E60">
         <f t="shared" ca="1" si="1"/>
-        <v>211670760</v>
+        <v>82473094</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -46052,7 +46182,7 @@
       </c>
       <c r="E61">
         <f t="shared" ca="1" si="1"/>
-        <v>184657176</v>
+        <v>196235967</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -46070,7 +46200,7 @@
       </c>
       <c r="E62">
         <f t="shared" ca="1" si="1"/>
-        <v>147247830</v>
+        <v>146760378</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -46088,7 +46218,7 @@
       </c>
       <c r="E63">
         <f t="shared" ca="1" si="1"/>
-        <v>220557760</v>
+        <v>76614741</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -46106,7 +46236,7 @@
       </c>
       <c r="E64">
         <f t="shared" ca="1" si="1"/>
-        <v>141924528</v>
+        <v>94274554</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -46124,7 +46254,7 @@
       </c>
       <c r="E65">
         <f t="shared" ca="1" si="1"/>
-        <v>194417832</v>
+        <v>200327985</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -46142,7 +46272,7 @@
       </c>
       <c r="E66">
         <f t="shared" ref="E66:E77" ca="1" si="2">RANDBETWEEN(50000,250000)*RANDBETWEEN(600,1200)</f>
-        <v>69406302</v>
+        <v>101323398</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -46160,7 +46290,7 @@
       </c>
       <c r="E67">
         <f t="shared" ca="1" si="2"/>
-        <v>94608600</v>
+        <v>191362050</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -46178,7 +46308,7 @@
       </c>
       <c r="E68">
         <f t="shared" ca="1" si="2"/>
-        <v>119224518</v>
+        <v>98571134</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -46196,7 +46326,7 @@
       </c>
       <c r="E69">
         <f t="shared" ca="1" si="2"/>
-        <v>85355440</v>
+        <v>292919595</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -46214,7 +46344,7 @@
       </c>
       <c r="E70">
         <f t="shared" ca="1" si="2"/>
-        <v>34589690</v>
+        <v>204913800</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -46232,7 +46362,7 @@
       </c>
       <c r="E71">
         <f t="shared" ca="1" si="2"/>
-        <v>72822105</v>
+        <v>135667840</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -46250,7 +46380,7 @@
       </c>
       <c r="E72">
         <f t="shared" ca="1" si="2"/>
-        <v>163476992</v>
+        <v>163614234</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -46268,7 +46398,7 @@
       </c>
       <c r="E73">
         <f t="shared" ca="1" si="2"/>
-        <v>57918536</v>
+        <v>156595257</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -46286,7 +46416,7 @@
       </c>
       <c r="E74">
         <f t="shared" ca="1" si="2"/>
-        <v>74036436</v>
+        <v>253264854</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -46304,7 +46434,7 @@
       </c>
       <c r="E75">
         <f t="shared" ca="1" si="2"/>
-        <v>74642400</v>
+        <v>281016200</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -46322,7 +46452,7 @@
       </c>
       <c r="E76">
         <f t="shared" ca="1" si="2"/>
-        <v>248238144</v>
+        <v>53939139</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -46340,7 +46470,7 @@
       </c>
       <c r="E77">
         <f t="shared" ca="1" si="2"/>
-        <v>136026150</v>
+        <v>117580280</v>
       </c>
     </row>
   </sheetData>

</xml_diff>